<commit_message>
Added missing payment from Ganesh Kumar
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,7 +830,9 @@
       <c r="D8" s="8">
         <v>200</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8">
+        <v>400</v>
+      </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -1489,7 +1491,7 @@
       </c>
       <c r="E35" s="8">
         <f t="shared" ref="E35:O35" si="0">SUM(E3:E34)</f>
-        <v>7000</v>
+        <v>7400</v>
       </c>
       <c r="F35" s="8">
         <f t="shared" si="0"/>
@@ -1533,7 +1535,7 @@
       </c>
       <c r="P35" s="2">
         <f>SUM(C35:O35)</f>
-        <v>12500</v>
+        <v>12900</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -1606,7 +1608,7 @@
       </c>
       <c r="E40" s="4">
         <f xml:space="preserve"> P35-D40</f>
-        <v>11235</v>
+        <v>11635</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -1624,7 +1626,7 @@
       </c>
       <c r="E41" s="4">
         <f>E40-D41</f>
-        <v>9985</v>
+        <v>10385</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -1642,7 +1644,7 @@
       </c>
       <c r="E42" s="4">
         <f t="shared" ref="E42:E52" si="1">E41-D42</f>
-        <v>8735</v>
+        <v>9135</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -1660,7 +1662,7 @@
       </c>
       <c r="E43" s="4">
         <f t="shared" si="1"/>
-        <v>7485</v>
+        <v>7885</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -1678,7 +1680,7 @@
       </c>
       <c r="E44" s="4">
         <f t="shared" si="1"/>
-        <v>6220</v>
+        <v>6620</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -1696,7 +1698,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>4955</v>
+        <v>5355</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -1708,7 +1710,7 @@
       <c r="D46" s="4"/>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>4955</v>
+        <v>5355</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -1720,7 +1722,7 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>4955</v>
+        <v>5355</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -1732,7 +1734,7 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>4955</v>
+        <v>5355</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1744,7 +1746,7 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>4955</v>
+        <v>5355</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1756,7 +1758,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>4955</v>
+        <v>5355</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1768,7 +1770,7 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>4955</v>
+        <v>5355</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1780,7 +1782,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>4955</v>
+        <v>5355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Kasi, Kasi paid 400 for May
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Ajun</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>24/05/2018, 7-8</t>
+  </si>
+  <si>
+    <t>Kasi</t>
   </si>
 </sst>
 </file>
@@ -613,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,12 +947,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="8">
-        <v>300</v>
-      </c>
+      <c r="D13" s="8"/>
       <c r="E13" s="8">
         <v>400</v>
       </c>
@@ -970,11 +971,15 @@
         <v>12</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="8">
+        <v>300</v>
+      </c>
+      <c r="E14" s="8">
+        <v>400</v>
+      </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -992,13 +997,11 @@
         <v>13</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="8">
-        <v>400</v>
-      </c>
+      <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1016,13 +1019,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="8">
-        <v>300</v>
-      </c>
-      <c r="E16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8">
+        <v>400</v>
+      </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -1040,15 +1043,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8">
         <v>300</v>
       </c>
-      <c r="E17" s="8">
-        <v>400</v>
-      </c>
+      <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -1066,7 +1067,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8">
@@ -1092,7 +1093,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8">
@@ -1118,11 +1119,15 @@
         <v>18</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="8">
+        <v>300</v>
+      </c>
+      <c r="E20" s="8">
+        <v>400</v>
+      </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -1140,15 +1145,11 @@
         <v>19</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="8">
-        <v>300</v>
-      </c>
-      <c r="E21" s="8">
-        <v>400</v>
-      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -1166,11 +1167,11 @@
         <v>20</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E22" s="8">
         <v>400</v>
@@ -1192,11 +1193,11 @@
         <v>21</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E23" s="8">
         <v>400</v>
@@ -1218,7 +1219,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8">
@@ -1244,11 +1245,15 @@
         <v>23</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="D25" s="8">
+        <v>300</v>
+      </c>
+      <c r="E25" s="8">
+        <v>400</v>
+      </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -1266,13 +1271,11 @@
         <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="8">
-        <v>400</v>
-      </c>
+      <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
@@ -1290,16 +1293,14 @@
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8">
         <v>400</v>
       </c>
-      <c r="F27" s="8">
-        <v>100</v>
-      </c>
+      <c r="F27" s="8"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
@@ -1316,16 +1317,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="D28" s="8">
-        <v>300</v>
-      </c>
+      <c r="D28" s="8"/>
       <c r="E28" s="8">
         <v>400</v>
       </c>
-      <c r="F28" s="8"/>
+      <c r="F28" s="8">
+        <v>100</v>
+      </c>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
@@ -1342,13 +1343,15 @@
         <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8">
         <v>300</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8">
+        <v>400</v>
+      </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
@@ -1366,10 +1369,12 @@
         <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="D30" s="8">
+        <v>300</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
@@ -1388,15 +1393,11 @@
         <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="8">
-        <v>300</v>
-      </c>
-      <c r="E31" s="8">
-        <v>400</v>
-      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -1414,7 +1415,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8">
@@ -1433,18 +1434,22 @@
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
       <c r="O32" s="8"/>
-      <c r="P32" s="12"/>
+      <c r="P32" s="9"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="D33" s="8">
+        <v>300</v>
+      </c>
+      <c r="E33" s="8">
+        <v>400</v>
+      </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
@@ -1455,331 +1460,353 @@
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
-      <c r="P33" s="2" t="s">
+      <c r="P33" s="12"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>32</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="2">
-        <f>SUM(D4:D33)</f>
+      <c r="B35" s="10"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="2">
+        <f>SUM(D4:D34)</f>
         <v>5400</v>
       </c>
-      <c r="E34" s="8">
-        <f t="shared" ref="E34:O34" si="0">SUM(E3:E33)</f>
-        <v>7900</v>
-      </c>
-      <c r="F34" s="8">
+      <c r="E35" s="8">
+        <f t="shared" ref="E35:O35" si="0">SUM(E3:E34)</f>
+        <v>8300</v>
+      </c>
+      <c r="F35" s="8">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G35" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H35" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I34" s="8">
+      <c r="I35" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J34" s="8">
+      <c r="J35" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K34" s="8">
+      <c r="K35" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L34" s="8">
+      <c r="L35" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M34" s="8">
+      <c r="M35" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N34" s="8">
+      <c r="N35" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O34" s="8">
+      <c r="O35" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P34" s="2">
-        <f>SUM(C34:O34)</f>
-        <v>13400</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-    </row>
-    <row r="37" spans="1:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="A37" s="14" t="s">
+      <c r="P35" s="2">
+        <f>SUM(C35:O35)</f>
+        <v>13800</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+    </row>
+    <row r="38" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="A38" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-    </row>
-    <row r="38" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+    </row>
+    <row r="39" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
-        <v>1</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="5">
-        <v>43200</v>
-      </c>
-      <c r="D39" s="4">
-        <v>1265</v>
-      </c>
-      <c r="E39" s="4">
-        <f xml:space="preserve"> P34-D39</f>
-        <v>12135</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C40" s="5">
-        <v>43207</v>
+        <v>43200</v>
       </c>
       <c r="D40" s="4">
-        <v>1250</v>
+        <v>1265</v>
       </c>
       <c r="E40" s="4">
-        <f>E39-D40</f>
-        <v>10885</v>
+        <f xml:space="preserve"> P35-D40</f>
+        <v>12535</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C41" s="5">
-        <v>43214</v>
+        <v>43207</v>
       </c>
       <c r="D41" s="4">
         <v>1250</v>
       </c>
       <c r="E41" s="4">
-        <f t="shared" ref="E41:E51" si="1">E40-D41</f>
-        <v>9635</v>
+        <f>E40-D41</f>
+        <v>11285</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42" s="5">
-        <v>43221</v>
+        <v>43214</v>
       </c>
       <c r="D42" s="4">
         <v>1250</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="1"/>
-        <v>8385</v>
+        <f t="shared" ref="E42:E52" si="1">E41-D42</f>
+        <v>10035</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C43" s="5">
-        <v>43227</v>
+        <v>43221</v>
       </c>
       <c r="D43" s="4">
-        <v>1265</v>
+        <v>1250</v>
       </c>
       <c r="E43" s="4">
         <f t="shared" si="1"/>
-        <v>7120</v>
+        <v>8785</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" s="5">
-        <v>43235</v>
+        <v>43227</v>
       </c>
       <c r="D44" s="4">
         <v>1265</v>
       </c>
       <c r="E44" s="4">
         <f t="shared" si="1"/>
-        <v>5855</v>
+        <v>7520</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="5">
-        <v>43241</v>
+        <v>43235</v>
       </c>
       <c r="D45" s="4">
         <v>1265</v>
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>4590</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
-        <v>8</v>
-      </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="5">
+        <v>43241</v>
+      </c>
+      <c r="D46" s="4">
+        <v>1265</v>
+      </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>4590</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>4590</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>4590</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>4590</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="6">
-        <v>12</v>
+      <c r="A50" s="4">
+        <v>11</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>4590</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>4590</v>
+        <v>4990</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="6">
+        <v>13</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4">
+        <f t="shared" si="1"/>
+        <v>4990</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B3:G33">
+  <sortState ref="B3:G34">
     <sortCondition ref="B3"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A37:P37"/>
+    <mergeCell ref="A38:P38"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:O33">
+  <conditionalFormatting sqref="A3:O34">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Enoch paid, Booked slot for 31May18
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>Ajun</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Kasi</t>
+  </si>
+  <si>
+    <t>31/05/2018, 6-7</t>
   </si>
 </sst>
 </file>
@@ -618,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A34"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,9 +811,11 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8">
-        <v>300</v>
-      </c>
-      <c r="F7" s="8"/>
+        <v>400</v>
+      </c>
+      <c r="F7" s="8">
+        <v>100</v>
+      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -1498,11 +1503,11 @@
       </c>
       <c r="E35" s="8">
         <f t="shared" ref="E35:O35" si="0">SUM(E3:E34)</f>
-        <v>8300</v>
+        <v>8400</v>
       </c>
       <c r="F35" s="8">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
@@ -1542,7 +1547,7 @@
       </c>
       <c r="P35" s="2">
         <f>SUM(C35:O35)</f>
-        <v>13800</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -1615,7 +1620,7 @@
       </c>
       <c r="E40" s="4">
         <f xml:space="preserve"> P35-D40</f>
-        <v>12535</v>
+        <v>12735</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -1633,7 +1638,7 @@
       </c>
       <c r="E41" s="4">
         <f>E40-D41</f>
-        <v>11285</v>
+        <v>11485</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -1651,7 +1656,7 @@
       </c>
       <c r="E42" s="4">
         <f t="shared" ref="E42:E52" si="1">E41-D42</f>
-        <v>10035</v>
+        <v>10235</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -1669,7 +1674,7 @@
       </c>
       <c r="E43" s="4">
         <f t="shared" si="1"/>
-        <v>8785</v>
+        <v>8985</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -1687,7 +1692,7 @@
       </c>
       <c r="E44" s="4">
         <f t="shared" si="1"/>
-        <v>7520</v>
+        <v>7720</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -1705,7 +1710,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>6255</v>
+        <v>6455</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -1723,19 +1728,25 @@
       </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>4990</v>
+        <v>5190</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>8</v>
       </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="5">
+        <v>43249</v>
+      </c>
+      <c r="D47" s="4">
+        <v>1265</v>
+      </c>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>4990</v>
+        <v>3925</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -1747,7 +1758,7 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>4990</v>
+        <v>3925</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1759,7 +1770,7 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>4990</v>
+        <v>3925</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1771,7 +1782,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>4990</v>
+        <v>3925</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1783,7 +1794,7 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>4990</v>
+        <v>3925</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1795,7 +1806,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>4990</v>
+        <v>3925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Booked slot for 07June18
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Ajun</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>31/05/2018, 6-7</t>
+  </si>
+  <si>
+    <t>07/06/2018, 6-7</t>
   </si>
 </sst>
 </file>
@@ -621,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1755,12 +1758,18 @@
       <c r="A48" s="4">
         <v>9</v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
+      <c r="B48" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="5">
+        <v>43256</v>
+      </c>
+      <c r="D48" s="4">
+        <v>1265</v>
+      </c>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>4025</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1772,7 +1781,7 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>4025</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1784,7 +1793,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>4025</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1796,7 +1805,7 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>4025</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1808,7 +1817,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>4025</v>
+        <v>2760</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
yogesh, vikram, vignesh, ganesh paid
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,7 +847,9 @@
       <c r="E8" s="8">
         <v>400</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8">
+        <v>300</v>
+      </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -1336,9 +1338,11 @@
         <v>400</v>
       </c>
       <c r="F28" s="8">
+        <v>300</v>
+      </c>
+      <c r="G28" s="8">
         <v>100</v>
       </c>
-      <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -1363,7 +1367,9 @@
       <c r="E29" s="8">
         <v>400</v>
       </c>
-      <c r="F29" s="8"/>
+      <c r="F29" s="8">
+        <v>300</v>
+      </c>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
@@ -1462,7 +1468,7 @@
         <v>400</v>
       </c>
       <c r="F33" s="8">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
@@ -1515,11 +1521,11 @@
       </c>
       <c r="F35" s="8">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>1300</v>
       </c>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H35" s="8">
         <f t="shared" si="0"/>
@@ -1555,7 +1561,7 @@
       </c>
       <c r="P35" s="2">
         <f>SUM(C35:O35)</f>
-        <v>14100</v>
+        <v>15200</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -1628,7 +1634,7 @@
       </c>
       <c r="E40" s="4">
         <f xml:space="preserve"> P35-D40</f>
-        <v>12835</v>
+        <v>13935</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -1646,7 +1652,7 @@
       </c>
       <c r="E41" s="4">
         <f>E40-D41</f>
-        <v>11585</v>
+        <v>12685</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -1664,7 +1670,7 @@
       </c>
       <c r="E42" s="4">
         <f t="shared" ref="E42:E52" si="1">E41-D42</f>
-        <v>10335</v>
+        <v>11435</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -1682,7 +1688,7 @@
       </c>
       <c r="E43" s="4">
         <f t="shared" si="1"/>
-        <v>9085</v>
+        <v>10185</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -1700,7 +1706,7 @@
       </c>
       <c r="E44" s="4">
         <f t="shared" si="1"/>
-        <v>7820</v>
+        <v>8920</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -1718,7 +1724,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>6555</v>
+        <v>7655</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -1736,7 +1742,7 @@
       </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>5290</v>
+        <v>6390</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -1754,7 +1760,7 @@
       </c>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>4025</v>
+        <v>5125</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -1772,7 +1778,7 @@
       </c>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>2760</v>
+        <v>3860</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1790,7 +1796,7 @@
       </c>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>1495</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1802,7 +1808,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>1495</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1814,7 +1820,7 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>1495</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1826,7 +1832,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>1495</v>
+        <v>2595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ganesh PK, Amar paid
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,7 +743,9 @@
       <c r="E4" s="8">
         <v>400</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="8">
+        <v>300</v>
+      </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -875,7 +877,9 @@
       <c r="E9" s="8">
         <v>400</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8">
+        <v>300</v>
+      </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -1521,7 +1525,7 @@
       </c>
       <c r="F35" s="8">
         <f t="shared" si="0"/>
-        <v>1300</v>
+        <v>1900</v>
       </c>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
@@ -1561,7 +1565,7 @@
       </c>
       <c r="P35" s="2">
         <f>SUM(C35:O35)</f>
-        <v>15200</v>
+        <v>15800</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -1634,7 +1638,7 @@
       </c>
       <c r="E40" s="4">
         <f xml:space="preserve"> P35-D40</f>
-        <v>13935</v>
+        <v>14535</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -1652,7 +1656,7 @@
       </c>
       <c r="E41" s="4">
         <f>E40-D41</f>
-        <v>12685</v>
+        <v>13285</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -1670,7 +1674,7 @@
       </c>
       <c r="E42" s="4">
         <f t="shared" ref="E42:E52" si="1">E41-D42</f>
-        <v>11435</v>
+        <v>12035</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -1688,7 +1692,7 @@
       </c>
       <c r="E43" s="4">
         <f t="shared" si="1"/>
-        <v>10185</v>
+        <v>10785</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -1706,7 +1710,7 @@
       </c>
       <c r="E44" s="4">
         <f t="shared" si="1"/>
-        <v>8920</v>
+        <v>9520</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -1724,7 +1728,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>7655</v>
+        <v>8255</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -1742,7 +1746,7 @@
       </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>6390</v>
+        <v>6990</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -1760,7 +1764,7 @@
       </c>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>5125</v>
+        <v>5725</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -1778,7 +1782,7 @@
       </c>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>3860</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1796,7 +1800,7 @@
       </c>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>2595</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1808,7 +1812,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>2595</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1820,7 +1824,7 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>2595</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1832,7 +1836,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>2595</v>
+        <v>3195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pravin, Shaiju and Tintu paid
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1043,7 +1043,9 @@
       <c r="E16" s="8">
         <v>400</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8">
+        <v>300</v>
+      </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1219,7 +1221,9 @@
       <c r="E23" s="8">
         <v>400</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="8">
+        <v>300</v>
+      </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -1271,7 +1275,9 @@
       <c r="E25" s="8">
         <v>400</v>
       </c>
-      <c r="F25" s="8"/>
+      <c r="F25" s="8">
+        <v>300</v>
+      </c>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
@@ -1527,7 +1533,7 @@
       </c>
       <c r="F35" s="8">
         <f t="shared" si="0"/>
-        <v>2200</v>
+        <v>3100</v>
       </c>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
@@ -1567,7 +1573,7 @@
       </c>
       <c r="P35" s="2">
         <f>SUM(C35:O35)</f>
-        <v>16100</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -1640,7 +1646,7 @@
       </c>
       <c r="E40" s="4">
         <f xml:space="preserve"> P35-D40</f>
-        <v>14835</v>
+        <v>15735</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -1658,7 +1664,7 @@
       </c>
       <c r="E41" s="4">
         <f>E40-D41</f>
-        <v>13585</v>
+        <v>14485</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -1676,7 +1682,7 @@
       </c>
       <c r="E42" s="4">
         <f t="shared" ref="E42:E52" si="1">E41-D42</f>
-        <v>12335</v>
+        <v>13235</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -1694,7 +1700,7 @@
       </c>
       <c r="E43" s="4">
         <f t="shared" si="1"/>
-        <v>11085</v>
+        <v>11985</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -1712,7 +1718,7 @@
       </c>
       <c r="E44" s="4">
         <f t="shared" si="1"/>
-        <v>9820</v>
+        <v>10720</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -1730,7 +1736,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>8555</v>
+        <v>9455</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -1748,7 +1754,7 @@
       </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>7290</v>
+        <v>8190</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -1766,7 +1772,7 @@
       </c>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>6025</v>
+        <v>6925</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -1784,7 +1790,7 @@
       </c>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>4760</v>
+        <v>5660</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1802,7 +1808,7 @@
       </c>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>3495</v>
+        <v>4395</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1814,7 +1820,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>3495</v>
+        <v>4395</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1826,7 +1832,7 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>3495</v>
+        <v>4395</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1838,7 +1844,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>3495</v>
+        <v>4395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
booked slot for 21st june 5-6
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>Ajun</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>13/06/2018, 6-7</t>
+  </si>
+  <si>
+    <t>21/06/2018, 5-6</t>
   </si>
 </sst>
 </file>
@@ -627,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1815,12 +1818,18 @@
       <c r="A50" s="4">
         <v>11</v>
       </c>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
+      <c r="B50" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="5">
+        <v>43269</v>
+      </c>
+      <c r="D50" s="4">
+        <v>1265</v>
+      </c>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>4395</v>
+        <v>3130</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1832,7 +1841,7 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>4395</v>
+        <v>3130</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1844,7 +1853,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>4395</v>
+        <v>3130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rk velu, jaga and shaiju paid
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Ajun</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>21/06/2018, 5-6</t>
+  </si>
+  <si>
+    <t>Jagatheesh</t>
   </si>
 </sst>
 </file>
@@ -628,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -991,16 +994,14 @@
         <v>12</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="8">
-        <v>300</v>
-      </c>
-      <c r="E14" s="8">
-        <v>400</v>
-      </c>
-      <c r="F14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8">
+        <v>300</v>
+      </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -1017,11 +1018,15 @@
         <v>13</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="8">
+        <v>300</v>
+      </c>
+      <c r="E15" s="8">
+        <v>400</v>
+      </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1039,16 +1044,12 @@
         <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="8">
-        <v>400</v>
-      </c>
-      <c r="F16" s="8">
-        <v>300</v>
-      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1065,14 +1066,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="8">
-        <v>300</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8">
+        <v>400</v>
+      </c>
+      <c r="F17" s="8">
+        <v>300</v>
+      </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -1089,15 +1092,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8">
         <v>300</v>
       </c>
-      <c r="E18" s="8">
-        <v>400</v>
-      </c>
+      <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -1115,7 +1116,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8">
@@ -1141,7 +1142,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8">
@@ -1150,7 +1151,9 @@
       <c r="E20" s="8">
         <v>400</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="8">
+        <v>300</v>
+      </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
@@ -1167,11 +1170,15 @@
         <v>19</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="D21" s="8">
+        <v>300</v>
+      </c>
+      <c r="E21" s="8">
+        <v>400</v>
+      </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -1189,15 +1196,11 @@
         <v>20</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="8">
-        <v>300</v>
-      </c>
-      <c r="E22" s="8">
-        <v>400</v>
-      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -1215,18 +1218,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E23" s="8">
         <v>400</v>
       </c>
-      <c r="F23" s="8">
-        <v>300</v>
-      </c>
+      <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -1243,17 +1244,21 @@
         <v>22</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E24" s="8">
         <v>400</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="F24" s="8">
+        <v>300</v>
+      </c>
+      <c r="G24" s="8">
+        <v>100</v>
+      </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -1269,7 +1274,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8">
@@ -1278,9 +1283,7 @@
       <c r="E25" s="8">
         <v>400</v>
       </c>
-      <c r="F25" s="8">
-        <v>300</v>
-      </c>
+      <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
@@ -1297,12 +1300,18 @@
         <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
+      <c r="D26" s="8">
+        <v>300</v>
+      </c>
+      <c r="E26" s="8">
+        <v>400</v>
+      </c>
+      <c r="F26" s="8">
+        <v>300</v>
+      </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
@@ -1319,13 +1328,11 @@
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="8">
-        <v>400</v>
-      </c>
+      <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
@@ -1343,19 +1350,15 @@
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8">
         <v>400</v>
       </c>
-      <c r="F28" s="8">
-        <v>300</v>
-      </c>
-      <c r="G28" s="8">
-        <v>100</v>
-      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -1371,19 +1374,19 @@
         <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="8"/>
-      <c r="D29" s="8">
-        <v>300</v>
-      </c>
+      <c r="D29" s="8"/>
       <c r="E29" s="8">
         <v>400</v>
       </c>
       <c r="F29" s="8">
         <v>300</v>
       </c>
-      <c r="G29" s="8"/>
+      <c r="G29" s="8">
+        <v>100</v>
+      </c>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
@@ -1399,14 +1402,18 @@
         <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8">
         <v>300</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
+      <c r="E30" s="8">
+        <v>400</v>
+      </c>
+      <c r="F30" s="8">
+        <v>300</v>
+      </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
@@ -1423,10 +1430,12 @@
         <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
+      <c r="D31" s="8">
+        <v>300</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
@@ -1445,18 +1454,12 @@
         <v>30</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C32" s="8"/>
-      <c r="D32" s="8">
-        <v>300</v>
-      </c>
-      <c r="E32" s="8">
-        <v>400</v>
-      </c>
-      <c r="F32" s="8">
-        <v>300</v>
-      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
@@ -1473,7 +1476,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8">
@@ -1494,19 +1497,25 @@
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
-      <c r="P33" s="12"/>
+      <c r="P33" s="9"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>32</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="D34" s="8">
+        <v>300</v>
+      </c>
+      <c r="E34" s="8">
+        <v>400</v>
+      </c>
+      <c r="F34" s="8">
+        <v>300</v>
+      </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
@@ -1516,355 +1525,377 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
-      <c r="P34" s="2" t="s">
+      <c r="P34" s="12"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>33</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="2">
-        <f>SUM(D4:D34)</f>
+      <c r="B36" s="10"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="2">
+        <f>SUM(D4:D35)</f>
         <v>5400</v>
       </c>
-      <c r="E35" s="8">
-        <f t="shared" ref="E35:O35" si="0">SUM(E3:E34)</f>
+      <c r="E36" s="8">
+        <f t="shared" ref="E36:O36" si="0">SUM(E3:E35)</f>
         <v>8400</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F36" s="8">
         <f t="shared" si="0"/>
-        <v>3100</v>
-      </c>
-      <c r="G35" s="8">
+        <v>3700</v>
+      </c>
+      <c r="G36" s="8">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="H35" s="8">
+        <v>200</v>
+      </c>
+      <c r="H36" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I36" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J35" s="8">
+      <c r="J36" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K35" s="8">
+      <c r="K36" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L35" s="8">
+      <c r="L36" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M35" s="8">
+      <c r="M36" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N35" s="8">
+      <c r="N36" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O35" s="8">
+      <c r="O36" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P35" s="2">
-        <f>SUM(C35:O35)</f>
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-    </row>
-    <row r="38" spans="1:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="A38" s="14" t="s">
+      <c r="P36" s="2">
+        <f>SUM(C36:O36)</f>
+        <v>17700</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+    </row>
+    <row r="39" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="A39" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-    </row>
-    <row r="39" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+    </row>
+    <row r="40" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
-        <v>1</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="5">
-        <v>43200</v>
-      </c>
-      <c r="D40" s="4">
-        <v>1265</v>
-      </c>
-      <c r="E40" s="4">
-        <f xml:space="preserve"> P35-D40</f>
-        <v>15735</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C41" s="5">
-        <v>43207</v>
+        <v>43200</v>
       </c>
       <c r="D41" s="4">
-        <v>1250</v>
+        <v>1265</v>
       </c>
       <c r="E41" s="4">
-        <f>E40-D41</f>
-        <v>14485</v>
+        <f xml:space="preserve"> P36-D41</f>
+        <v>16435</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C42" s="5">
-        <v>43214</v>
+        <v>43207</v>
       </c>
       <c r="D42" s="4">
         <v>1250</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" ref="E42:E52" si="1">E41-D42</f>
-        <v>13235</v>
+        <f>E41-D42</f>
+        <v>15185</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" s="5">
-        <v>43221</v>
+        <v>43214</v>
       </c>
       <c r="D43" s="4">
         <v>1250</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" si="1"/>
-        <v>11985</v>
+        <f t="shared" ref="E43:E53" si="1">E42-D43</f>
+        <v>13935</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C44" s="5">
-        <v>43227</v>
+        <v>43221</v>
       </c>
       <c r="D44" s="4">
-        <v>1265</v>
+        <v>1250</v>
       </c>
       <c r="E44" s="4">
         <f t="shared" si="1"/>
-        <v>10720</v>
+        <v>12685</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" s="5">
-        <v>43235</v>
+        <v>43227</v>
       </c>
       <c r="D45" s="4">
         <v>1265</v>
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>9455</v>
+        <v>11420</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46" s="5">
-        <v>43241</v>
+        <v>43235</v>
       </c>
       <c r="D46" s="4">
         <v>1265</v>
       </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>8190</v>
+        <v>10155</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C47" s="5">
-        <v>43249</v>
+        <v>43241</v>
       </c>
       <c r="D47" s="4">
         <v>1265</v>
       </c>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>6925</v>
+        <v>8890</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" s="5">
-        <v>43256</v>
+        <v>43249</v>
       </c>
       <c r="D48" s="4">
         <v>1265</v>
       </c>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>5660</v>
+        <v>7625</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" s="5">
-        <v>43262</v>
+        <v>43256</v>
       </c>
       <c r="D49" s="4">
         <v>1265</v>
       </c>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>4395</v>
+        <v>6360</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C50" s="5">
-        <v>43269</v>
+        <v>43262</v>
       </c>
       <c r="D50" s="4">
         <v>1265</v>
       </c>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>3130</v>
+        <v>5095</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="6">
-        <v>12</v>
-      </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
+      <c r="A51" s="4">
+        <v>11</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="5">
+        <v>43269</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1265</v>
+      </c>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>3130</v>
+        <v>3830</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>3130</v>
+        <v>3830</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="6">
+        <v>13</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4">
+        <f t="shared" si="1"/>
+        <v>3830</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B3:G34">
+  <sortState ref="B3:G35">
     <sortCondition ref="B3"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A38:P38"/>
+    <mergeCell ref="A39:P39"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:O34">
+  <conditionalFormatting sqref="A3:O35">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
George paid, slot booked for 26thJune
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>Ajun</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>Jagatheesh</t>
+  </si>
+  <si>
+    <t>26/06/2018, 4-5</t>
   </si>
 </sst>
 </file>
@@ -633,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,7 +910,9 @@
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8">
+        <v>300</v>
+      </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -1567,7 +1572,7 @@
       </c>
       <c r="F36" s="8">
         <f t="shared" si="0"/>
-        <v>3700</v>
+        <v>4000</v>
       </c>
       <c r="G36" s="8">
         <f t="shared" si="0"/>
@@ -1607,7 +1612,7 @@
       </c>
       <c r="P36" s="2">
         <f>SUM(C36:O36)</f>
-        <v>17700</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
@@ -1680,7 +1685,7 @@
       </c>
       <c r="E41" s="4">
         <f xml:space="preserve"> P36-D41</f>
-        <v>16435</v>
+        <v>16735</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -1698,7 +1703,7 @@
       </c>
       <c r="E42" s="4">
         <f>E41-D42</f>
-        <v>15185</v>
+        <v>15485</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -1716,7 +1721,7 @@
       </c>
       <c r="E43" s="4">
         <f t="shared" ref="E43:E53" si="1">E42-D43</f>
-        <v>13935</v>
+        <v>14235</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -1734,7 +1739,7 @@
       </c>
       <c r="E44" s="4">
         <f t="shared" si="1"/>
-        <v>12685</v>
+        <v>12985</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -1752,7 +1757,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>11420</v>
+        <v>11720</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -1770,7 +1775,7 @@
       </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>10155</v>
+        <v>10455</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -1788,7 +1793,7 @@
       </c>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>8890</v>
+        <v>9190</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -1806,7 +1811,7 @@
       </c>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>7625</v>
+        <v>7925</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1824,7 +1829,7 @@
       </c>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>6360</v>
+        <v>6660</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1842,7 +1847,7 @@
       </c>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>5095</v>
+        <v>5395</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1860,19 +1865,25 @@
       </c>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>3830</v>
+        <v>4130</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>12</v>
       </c>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
+      <c r="B52" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="5">
+        <v>43277</v>
+      </c>
+      <c r="D52" s="4">
+        <v>1265</v>
+      </c>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>3830</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1884,7 +1895,7 @@
       <c r="D53" s="4"/>
       <c r="E53" s="4">
         <f t="shared" si="1"/>
-        <v>3830</v>
+        <v>2865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bookded slot for 28Jun
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>Ajun</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>26/06/2018, 4-5</t>
+  </si>
+  <si>
+    <t>28/06/2018, 4-5</t>
   </si>
 </sst>
 </file>
@@ -637,7 +640,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1890,12 +1893,18 @@
       <c r="A53" s="6">
         <v>13</v>
       </c>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
+      <c r="B53" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="5">
+        <v>43278</v>
+      </c>
+      <c r="D53" s="4">
+        <v>1265</v>
+      </c>
       <c r="E53" s="4">
         <f t="shared" si="1"/>
-        <v>2865</v>
+        <v>1600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slots booked for 3rd and 5th July
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Ajun</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>Kailash</t>
+  </si>
+  <si>
+    <t>03/07/2018, 5-6</t>
+  </si>
+  <si>
+    <t>05/07/2018, 6-7</t>
   </si>
 </sst>
 </file>
@@ -281,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -304,11 +310,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -351,6 +368,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -640,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1005,7 +1025,9 @@
       <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
       <c r="B14" s="11" t="s">
         <v>69</v>
       </c>
@@ -1030,7 +1052,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>66</v>
@@ -1054,7 +1076,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>10</v>
@@ -1080,7 +1102,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>26</v>
@@ -1102,7 +1124,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>11</v>
@@ -1128,7 +1150,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>13</v>
@@ -1152,7 +1174,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>4</v>
@@ -1178,7 +1200,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>57</v>
@@ -1206,7 +1228,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>5</v>
@@ -1232,7 +1254,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>14</v>
@@ -1254,7 +1276,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>15</v>
@@ -1280,7 +1302,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>53</v>
@@ -1310,7 +1332,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>16</v>
@@ -1336,7 +1358,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>27</v>
@@ -1364,7 +1386,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>17</v>
@@ -1386,7 +1408,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>22</v>
@@ -1410,7 +1432,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>18</v>
@@ -1438,7 +1460,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>19</v>
@@ -1466,7 +1488,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>20</v>
@@ -1490,7 +1512,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>21</v>
@@ -1512,7 +1534,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>6</v>
@@ -1540,7 +1562,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>7</v>
@@ -1568,7 +1590,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>8</v>
@@ -1601,47 +1623,47 @@
         <v>5400</v>
       </c>
       <c r="E37" s="8">
-        <f>SUM(E3:E36)</f>
+        <f t="shared" ref="E37:O37" si="0">SUM(E3:E36)</f>
         <v>8400</v>
       </c>
       <c r="F37" s="8">
-        <f>SUM(F3:F36)</f>
+        <f t="shared" si="0"/>
         <v>4400</v>
       </c>
       <c r="G37" s="8">
-        <f>SUM(G3:G36)</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="H37" s="8">
-        <f>SUM(H3:H36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I37" s="8">
-        <f>SUM(I3:I36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J37" s="8">
-        <f>SUM(J3:J36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K37" s="8">
-        <f>SUM(K3:K36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L37" s="8">
-        <f>SUM(L3:L36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M37" s="8">
-        <f>SUM(M3:M36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N37" s="8">
-        <f>SUM(N3:N36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O37" s="8">
-        <f>SUM(O3:O36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P37" s="2">
@@ -1754,7 +1776,7 @@
         <v>1250</v>
       </c>
       <c r="E44" s="4">
-        <f t="shared" ref="E44:E54" si="0">E43-D44</f>
+        <f t="shared" ref="E44:E54" si="1">E43-D44</f>
         <v>15435</v>
       </c>
     </row>
@@ -1772,7 +1794,7 @@
         <v>1250</v>
       </c>
       <c r="E45" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14185</v>
       </c>
     </row>
@@ -1790,7 +1812,7 @@
         <v>1265</v>
       </c>
       <c r="E46" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12920</v>
       </c>
     </row>
@@ -1808,7 +1830,7 @@
         <v>1265</v>
       </c>
       <c r="E47" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11655</v>
       </c>
     </row>
@@ -1826,7 +1848,7 @@
         <v>1265</v>
       </c>
       <c r="E48" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10390</v>
       </c>
     </row>
@@ -1844,7 +1866,7 @@
         <v>1265</v>
       </c>
       <c r="E49" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9125</v>
       </c>
     </row>
@@ -1862,7 +1884,7 @@
         <v>1265</v>
       </c>
       <c r="E50" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7860</v>
       </c>
     </row>
@@ -1880,7 +1902,7 @@
         <v>1265</v>
       </c>
       <c r="E51" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6595</v>
       </c>
     </row>
@@ -1898,7 +1920,7 @@
         <v>1265</v>
       </c>
       <c r="E52" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5330</v>
       </c>
     </row>
@@ -1916,7 +1938,7 @@
         <v>1265</v>
       </c>
       <c r="E53" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4065</v>
       </c>
     </row>
@@ -1934,9 +1956,135 @@
         <v>1265</v>
       </c>
       <c r="E54" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2800</v>
       </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="15">
+        <v>14</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="5">
+        <v>43279</v>
+      </c>
+      <c r="D55" s="6">
+        <v>1265</v>
+      </c>
+      <c r="E55" s="6">
+        <f>E54-D55</f>
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="6">
+        <v>15</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="5">
+        <v>43279</v>
+      </c>
+      <c r="D56" s="6">
+        <v>1265</v>
+      </c>
+      <c r="E56" s="6">
+        <f>E55-D56</f>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="6">
+        <v>16</v>
+      </c>
+      <c r="B57" s="6"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="15">
+        <v>17</v>
+      </c>
+      <c r="B58" s="6"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="6">
+        <v>18</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="6">
+        <v>19</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="15">
+        <v>20</v>
+      </c>
+      <c r="B61" s="6"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="6">
+        <v>21</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="6">
+        <v>22</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="15">
+        <v>23</v>
+      </c>
+      <c r="B64" s="6"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="6">
+        <v>24</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="6">
+        <v>25</v>
+      </c>
+      <c r="B66" s="6"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
     </row>
   </sheetData>
   <sortState ref="B3:G36">

</xml_diff>

<commit_message>
correction for Enoch's payment
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,10 +859,10 @@
         <v>400</v>
       </c>
       <c r="F7" s="8">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="G7" s="8">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -1632,11 +1632,11 @@
       </c>
       <c r="F37" s="8">
         <f t="shared" si="0"/>
-        <v>4700</v>
+        <v>4900</v>
       </c>
       <c r="G37" s="8">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="H37" s="8">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Aniket, Vikram, Riyas, Tintu and Athul Paid
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -663,7 +663,7 @@
   <dimension ref="A1:P66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,7 +806,9 @@
       <c r="E5" s="8">
         <v>400</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8">
+        <v>300</v>
+      </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -835,7 +837,9 @@
       <c r="F6" s="8">
         <v>300</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="8">
+        <v>500</v>
+      </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -1191,7 +1195,9 @@
         <v>400</v>
       </c>
       <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="G20" s="8">
+        <v>500</v>
+      </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -1381,7 +1387,9 @@
       <c r="F27" s="8">
         <v>300</v>
       </c>
-      <c r="G27" s="8"/>
+      <c r="G27" s="8">
+        <v>500</v>
+      </c>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
@@ -1484,7 +1492,7 @@
         <v>300</v>
       </c>
       <c r="G31" s="8">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
@@ -1638,11 +1646,11 @@
       </c>
       <c r="F37" s="8">
         <f t="shared" si="0"/>
-        <v>5200</v>
+        <v>5500</v>
       </c>
       <c r="G37" s="8">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>3100</v>
       </c>
       <c r="H37" s="8">
         <f t="shared" si="0"/>
@@ -1678,7 +1686,7 @@
       </c>
       <c r="P37" s="2">
         <f>SUM(C37:O37)</f>
-        <v>20500</v>
+        <v>22400</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -1751,7 +1759,7 @@
       </c>
       <c r="E42" s="4">
         <f xml:space="preserve"> P37-D42</f>
-        <v>19235</v>
+        <v>21135</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -1769,7 +1777,7 @@
       </c>
       <c r="E43" s="4">
         <f>E42-D43</f>
-        <v>17985</v>
+        <v>19885</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -1787,7 +1795,7 @@
       </c>
       <c r="E44" s="4">
         <f t="shared" ref="E44:E54" si="1">E43-D44</f>
-        <v>16735</v>
+        <v>18635</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -1805,7 +1813,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>15485</v>
+        <v>17385</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -1823,7 +1831,7 @@
       </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>14220</v>
+        <v>16120</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -1841,7 +1849,7 @@
       </c>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>12955</v>
+        <v>14855</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -1859,7 +1867,7 @@
       </c>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>11690</v>
+        <v>13590</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1877,7 +1885,7 @@
       </c>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>10425</v>
+        <v>12325</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1895,7 +1903,7 @@
       </c>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>9160</v>
+        <v>11060</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1913,7 +1921,7 @@
       </c>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>7895</v>
+        <v>9795</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1931,7 +1939,7 @@
       </c>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>6630</v>
+        <v>8530</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1949,7 +1957,7 @@
       </c>
       <c r="E53" s="4">
         <f t="shared" si="1"/>
-        <v>5365</v>
+        <v>7265</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1967,7 +1975,7 @@
       </c>
       <c r="E54" s="4">
         <f t="shared" si="1"/>
-        <v>4100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1985,7 +1993,7 @@
       </c>
       <c r="E55" s="6">
         <f>E54-D55</f>
-        <v>2835</v>
+        <v>4735</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2003,7 +2011,7 @@
       </c>
       <c r="E56" s="6">
         <f>E55-D56</f>
-        <v>1570</v>
+        <v>3470</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Enoch, Vishnu, Ganesh and George paid
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,7 +866,7 @@
         <v>300</v>
       </c>
       <c r="G7" s="8">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -895,7 +895,9 @@
       <c r="F8" s="8">
         <v>300</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="8">
+        <v>500</v>
+      </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -947,7 +949,9 @@
       <c r="F10" s="8">
         <v>300</v>
       </c>
-      <c r="G10" s="8"/>
+      <c r="G10" s="8">
+        <v>500</v>
+      </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -1567,7 +1571,9 @@
       <c r="F34" s="8">
         <v>300</v>
       </c>
-      <c r="G34" s="8"/>
+      <c r="G34" s="8">
+        <v>500</v>
+      </c>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
@@ -1652,7 +1658,7 @@
       </c>
       <c r="G37" s="8">
         <f t="shared" si="0"/>
-        <v>3600</v>
+        <v>5400</v>
       </c>
       <c r="H37" s="8">
         <f t="shared" si="0"/>
@@ -1688,7 +1694,7 @@
       </c>
       <c r="P37" s="2">
         <f>SUM(C37:O37)</f>
-        <v>22900</v>
+        <v>24700</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -1761,7 +1767,7 @@
       </c>
       <c r="E42" s="4">
         <f xml:space="preserve"> P37-D42</f>
-        <v>21635</v>
+        <v>23435</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -1779,7 +1785,7 @@
       </c>
       <c r="E43" s="4">
         <f>E42-D43</f>
-        <v>20385</v>
+        <v>22185</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -1797,7 +1803,7 @@
       </c>
       <c r="E44" s="4">
         <f t="shared" ref="E44:E54" si="1">E43-D44</f>
-        <v>19135</v>
+        <v>20935</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -1815,7 +1821,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>17885</v>
+        <v>19685</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -1833,7 +1839,7 @@
       </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>16620</v>
+        <v>18420</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -1851,7 +1857,7 @@
       </c>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>15355</v>
+        <v>17155</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -1869,7 +1875,7 @@
       </c>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>14090</v>
+        <v>15890</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1887,7 +1893,7 @@
       </c>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>12825</v>
+        <v>14625</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1905,7 +1911,7 @@
       </c>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>11560</v>
+        <v>13360</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1923,7 +1929,7 @@
       </c>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>10295</v>
+        <v>12095</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1941,7 +1947,7 @@
       </c>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>9030</v>
+        <v>10830</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1959,7 +1965,7 @@
       </c>
       <c r="E53" s="4">
         <f t="shared" si="1"/>
-        <v>7765</v>
+        <v>9565</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1977,7 +1983,7 @@
       </c>
       <c r="E54" s="4">
         <f t="shared" si="1"/>
-        <v>6500</v>
+        <v>8300</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1995,7 +2001,7 @@
       </c>
       <c r="E55" s="6">
         <f>E54-D55</f>
-        <v>5235</v>
+        <v>7035</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2013,7 +2019,7 @@
       </c>
       <c r="E56" s="6">
         <f>E55-D56</f>
-        <v>3970</v>
+        <v>5770</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ganesh and Amar paid
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -663,7 +663,7 @@
   <dimension ref="A1:P66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,7 +781,9 @@
       <c r="F4" s="8">
         <v>300</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="8">
+        <v>500</v>
+      </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -925,7 +927,9 @@
       <c r="F9" s="8">
         <v>300</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="8">
+        <v>500</v>
+      </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -1658,7 +1662,7 @@
       </c>
       <c r="G37" s="8">
         <f t="shared" si="0"/>
-        <v>5400</v>
+        <v>6400</v>
       </c>
       <c r="H37" s="8">
         <f t="shared" si="0"/>
@@ -1694,7 +1698,7 @@
       </c>
       <c r="P37" s="2">
         <f>SUM(C37:O37)</f>
-        <v>24700</v>
+        <v>25700</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -1767,7 +1771,7 @@
       </c>
       <c r="E42" s="4">
         <f xml:space="preserve"> P37-D42</f>
-        <v>23435</v>
+        <v>24435</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -1785,7 +1789,7 @@
       </c>
       <c r="E43" s="4">
         <f>E42-D43</f>
-        <v>22185</v>
+        <v>23185</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -1803,7 +1807,7 @@
       </c>
       <c r="E44" s="4">
         <f t="shared" ref="E44:E54" si="1">E43-D44</f>
-        <v>20935</v>
+        <v>21935</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -1821,7 +1825,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>19685</v>
+        <v>20685</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -1839,7 +1843,7 @@
       </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>18420</v>
+        <v>19420</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -1857,7 +1861,7 @@
       </c>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>17155</v>
+        <v>18155</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -1875,7 +1879,7 @@
       </c>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>15890</v>
+        <v>16890</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1893,7 +1897,7 @@
       </c>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>14625</v>
+        <v>15625</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1911,7 +1915,7 @@
       </c>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>13360</v>
+        <v>14360</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1929,7 +1933,7 @@
       </c>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>12095</v>
+        <v>13095</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1947,7 +1951,7 @@
       </c>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>10830</v>
+        <v>11830</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1965,7 +1969,7 @@
       </c>
       <c r="E53" s="4">
         <f t="shared" si="1"/>
-        <v>9565</v>
+        <v>10565</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1983,7 +1987,7 @@
       </c>
       <c r="E54" s="4">
         <f t="shared" si="1"/>
-        <v>8300</v>
+        <v>9300</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -2001,7 +2005,7 @@
       </c>
       <c r="E55" s="6">
         <f>E54-D55</f>
-        <v>7035</v>
+        <v>8035</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2019,7 +2023,7 @@
       </c>
       <c r="E56" s="6">
         <f>E55-D56</f>
-        <v>5770</v>
+        <v>6770</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
pravin, sadik, Aniket paid
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,7 +811,9 @@
       <c r="F5" s="8">
         <v>300</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="8">
+        <v>500</v>
+      </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -1153,7 +1155,9 @@
       <c r="F18" s="8">
         <v>300</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="8">
+        <v>500</v>
+      </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -1259,7 +1263,9 @@
         <v>400</v>
       </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="G22" s="8">
+        <v>500</v>
+      </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -1662,7 +1668,7 @@
       </c>
       <c r="G37" s="8">
         <f t="shared" si="0"/>
-        <v>6400</v>
+        <v>7900</v>
       </c>
       <c r="H37" s="8">
         <f t="shared" si="0"/>
@@ -1698,7 +1704,7 @@
       </c>
       <c r="P37" s="2">
         <f>SUM(C37:O37)</f>
-        <v>25700</v>
+        <v>27200</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -1771,7 +1777,7 @@
       </c>
       <c r="E42" s="4">
         <f xml:space="preserve"> P37-D42</f>
-        <v>24435</v>
+        <v>25935</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -1789,7 +1795,7 @@
       </c>
       <c r="E43" s="4">
         <f>E42-D43</f>
-        <v>23185</v>
+        <v>24685</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -1807,7 +1813,7 @@
       </c>
       <c r="E44" s="4">
         <f t="shared" ref="E44:E54" si="1">E43-D44</f>
-        <v>21935</v>
+        <v>23435</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -1825,7 +1831,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>20685</v>
+        <v>22185</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -1843,7 +1849,7 @@
       </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>19420</v>
+        <v>20920</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -1861,7 +1867,7 @@
       </c>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>18155</v>
+        <v>19655</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -1879,7 +1885,7 @@
       </c>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>16890</v>
+        <v>18390</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1897,7 +1903,7 @@
       </c>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>15625</v>
+        <v>17125</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1915,7 +1921,7 @@
       </c>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>14360</v>
+        <v>15860</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,7 +1939,7 @@
       </c>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>13095</v>
+        <v>14595</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1951,7 +1957,7 @@
       </c>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>11830</v>
+        <v>13330</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1969,7 +1975,7 @@
       </c>
       <c r="E53" s="4">
         <f t="shared" si="1"/>
-        <v>10565</v>
+        <v>12065</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1987,7 +1993,7 @@
       </c>
       <c r="E54" s="4">
         <f t="shared" si="1"/>
-        <v>9300</v>
+        <v>10800</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -2005,7 +2011,7 @@
       </c>
       <c r="E55" s="6">
         <f>E54-D55</f>
-        <v>8035</v>
+        <v>9535</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2023,7 +2029,7 @@
       </c>
       <c r="E56" s="6">
         <f>E55-D56</f>
-        <v>6770</v>
+        <v>8270</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Justin and Shaiju paid
</commit_message>
<xml_diff>
--- a/MCHP_Football_Fund.xlsx
+++ b/MCHP_Football_Fund.xlsx
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1106,7 +1106,7 @@
         <v>300</v>
       </c>
       <c r="G16" s="8">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1342,7 +1342,7 @@
         <v>300</v>
       </c>
       <c r="G25" s="8">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
@@ -1668,7 +1668,7 @@
       </c>
       <c r="G37" s="8">
         <f t="shared" si="0"/>
-        <v>7900</v>
+        <v>8700</v>
       </c>
       <c r="H37" s="8">
         <f t="shared" si="0"/>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="P37" s="2">
         <f>SUM(C37:O37)</f>
-        <v>27200</v>
+        <v>28000</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="E42" s="4">
         <f xml:space="preserve"> P37-D42</f>
-        <v>25935</v>
+        <v>26735</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -1795,7 +1795,7 @@
       </c>
       <c r="E43" s="4">
         <f>E42-D43</f>
-        <v>24685</v>
+        <v>25485</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="E44" s="4">
         <f t="shared" ref="E44:E54" si="1">E43-D44</f>
-        <v>23435</v>
+        <v>24235</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="1"/>
-        <v>22185</v>
+        <v>22985</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -1849,7 +1849,7 @@
       </c>
       <c r="E46" s="4">
         <f t="shared" si="1"/>
-        <v>20920</v>
+        <v>21720</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="E47" s="4">
         <f t="shared" si="1"/>
-        <v>19655</v>
+        <v>20455</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="E48" s="4">
         <f t="shared" si="1"/>
-        <v>18390</v>
+        <v>19190</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="E49" s="4">
         <f t="shared" si="1"/>
-        <v>17125</v>
+        <v>17925</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="E50" s="4">
         <f t="shared" si="1"/>
-        <v>15860</v>
+        <v>16660</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1939,7 +1939,7 @@
       </c>
       <c r="E51" s="4">
         <f t="shared" si="1"/>
-        <v>14595</v>
+        <v>15395</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="E52" s="4">
         <f t="shared" si="1"/>
-        <v>13330</v>
+        <v>14130</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1975,7 +1975,7 @@
       </c>
       <c r="E53" s="4">
         <f t="shared" si="1"/>
-        <v>12065</v>
+        <v>12865</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="E54" s="4">
         <f t="shared" si="1"/>
-        <v>10800</v>
+        <v>11600</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="E55" s="6">
         <f>E54-D55</f>
-        <v>9535</v>
+        <v>10335</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="E56" s="6">
         <f>E55-D56</f>
-        <v>8270</v>
+        <v>9070</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>